<commit_message>
Update binary data files for interest rates bootstrap project
</commit_message>
<xml_diff>
--- a/projects/2-interest-rates-bootstrap/data/raw/MktData_CurveBootstrap.xlsx
+++ b/projects/2-interest-rates-bootstrap/data/raw/MktData_CurveBootstrap.xlsx
@@ -115,7 +115,7 @@
     <numFmt numFmtId="165" formatCode="#,##0.000"/>
     <numFmt numFmtId="166" formatCode="#,##0.00000"/>
   </numFmts>
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -150,7 +150,7 @@
     </font>
     <font>
       <sz val="10"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Century Gothic"/>
       <family val="2"/>
     </font>
@@ -208,7 +208,7 @@
     <font>
       <b/>
       <sz val="10"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Century Gothic"/>
       <family val="2"/>
     </font>
@@ -226,13 +226,19 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -270,7 +276,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="42">
+  <borders count="43">
     <border>
       <left/>
       <right/>
@@ -849,6 +855,13 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FFc6c6c6"/>
       </left>
@@ -897,7 +910,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="155">
+  <cellXfs count="157">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1277,77 +1290,83 @@
     <xf xfId="0" numFmtId="165" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="17" applyFont="1" fillId="4" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf xfId="0" numFmtId="1" applyNumberFormat="1" borderId="39" applyBorder="1" fontId="18" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="39" applyBorder="1" fontId="18" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="15" applyNumberFormat="1" borderId="40" applyBorder="1" fontId="5" applyFont="1" fillId="5" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf xfId="0" numFmtId="166" applyNumberFormat="1" borderId="41" applyBorder="1" fontId="5" applyFont="1" fillId="5" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf xfId="0" numFmtId="15" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="17" applyFont="1" fillId="4" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="166" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="17" applyFont="1" fillId="4" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="166" applyNumberFormat="1" borderId="39" applyBorder="1" fontId="18" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="165" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="5" applyFont="1" fillId="4" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf xfId="0" numFmtId="165" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="17" applyFont="1" fillId="4" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="19" applyFont="1" fillId="4" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="1" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="19" applyFont="1" fillId="4" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="166" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="19" applyFont="1" fillId="4" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="15" applyNumberFormat="1" borderId="42" applyBorder="1" fontId="5" applyFont="1" fillId="4" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="6" applyFont="1" fillId="4" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf xfId="0" numFmtId="15" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="5" applyFont="1" fillId="4" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="14" applyFont="1" fillId="4" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="17" applyFont="1" fillId="4" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="165" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="17" applyFont="1" fillId="4" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="165" applyNumberFormat="1" borderId="39" applyBorder="1" fontId="18" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="39" applyBorder="1" fontId="18" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general"/>
+    </xf>
     <xf xfId="0" numFmtId="1" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="15" applyNumberFormat="1" borderId="39" applyBorder="1" fontId="5" applyFont="1" fillId="5" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf xfId="0" numFmtId="166" applyNumberFormat="1" borderId="40" applyBorder="1" fontId="5" applyFont="1" fillId="5" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf xfId="0" numFmtId="15" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="17" applyFont="1" fillId="4" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="166" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="17" applyFont="1" fillId="4" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf xfId="0" numFmtId="166" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="165" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="5" applyFont="1" fillId="4" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf xfId="0" numFmtId="165" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="17" applyFont="1" fillId="4" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="18" applyFont="1" fillId="4" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="1" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="18" applyFont="1" fillId="4" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="166" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="18" applyFont="1" fillId="4" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="15" applyNumberFormat="1" borderId="41" applyBorder="1" fontId="5" applyFont="1" fillId="4" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="6" applyFont="1" fillId="4" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf xfId="0" numFmtId="15" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="5" applyFont="1" fillId="4" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="14" applyFont="1" fillId="4" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="17" applyFont="1" fillId="4" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="165" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="17" applyFont="1" fillId="4" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="165" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
     <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="1" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="165" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="165" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
@@ -1675,20 +1694,20 @@
     <col min="4" max="4" style="149" width="13.290714285714287" customWidth="1" bestFit="1"/>
     <col min="5" max="5" style="150" width="10.576428571428572" customWidth="1" bestFit="1"/>
     <col min="6" max="6" style="150" width="9.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="147" width="9.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="151" width="9.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="9" max="9" style="151" width="9.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="151" width="9.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="152" width="9.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="9" max="9" style="153" width="9.147857142857141" customWidth="1" bestFit="1"/>
     <col min="10" max="10" style="147" width="9.147857142857141" customWidth="1" bestFit="1"/>
     <col min="11" max="11" style="148" width="9.147857142857141" customWidth="1" bestFit="1"/>
     <col min="12" max="12" style="149" width="9.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="13" max="13" style="152" width="9.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="13" max="13" style="154" width="9.147857142857141" customWidth="1" bestFit="1"/>
     <col min="14" max="14" style="147" width="9.147857142857141" customWidth="1" bestFit="1"/>
     <col min="15" max="15" style="148" width="4.719285714285714" customWidth="1" bestFit="1"/>
     <col min="16" max="16" style="149" width="10.43357142857143" customWidth="1" bestFit="1"/>
     <col min="17" max="17" style="149" width="10.290714285714287" customWidth="1" bestFit="1"/>
     <col min="18" max="18" style="149" width="10.290714285714287" customWidth="1" bestFit="1"/>
-    <col min="19" max="19" style="153" width="9.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="20" max="20" style="154" width="9.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="19" max="19" style="155" width="9.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="20" max="20" style="156" width="9.147857142857141" customWidth="1" bestFit="1"/>
     <col min="21" max="21" style="148" width="18.862142857142857" customWidth="1" bestFit="1"/>
     <col min="22" max="22" style="147" width="13.576428571428572" customWidth="1" bestFit="1"/>
     <col min="23" max="23" style="147" width="13.576428571428572" customWidth="1" bestFit="1"/>
@@ -4847,7 +4866,7 @@
       <c r="Z75" s="7"/>
       <c r="AA75" s="7"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="76" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="76" customHeight="1" ht="20.25">
       <c r="A76" s="7"/>
       <c r="B76" s="54">
         <v>38</v>
@@ -5093,7 +5112,7 @@
       <c r="Z81" s="7"/>
       <c r="AA81" s="7"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="82" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="82" customHeight="1" ht="19.5">
       <c r="A82" s="7"/>
       <c r="B82" s="54">
         <v>44</v>
@@ -5134,7 +5153,7 @@
       <c r="Z82" s="7"/>
       <c r="AA82" s="7"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="83" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="83" customHeight="1" ht="19.5">
       <c r="A83" s="7"/>
       <c r="B83" s="54">
         <v>45</v>
@@ -5175,7 +5194,7 @@
       <c r="Z83" s="7"/>
       <c r="AA83" s="7"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="84" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="84" customHeight="1" ht="19.5">
       <c r="A84" s="7"/>
       <c r="B84" s="54">
         <v>46</v>
@@ -5216,7 +5235,7 @@
       <c r="Z84" s="7"/>
       <c r="AA84" s="7"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="85" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="85" customHeight="1" ht="19.5">
       <c r="A85" s="7"/>
       <c r="B85" s="54">
         <v>47</v>
@@ -5257,7 +5276,7 @@
       <c r="Z85" s="7"/>
       <c r="AA85" s="7"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="86" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="86" customHeight="1" ht="19.5">
       <c r="A86" s="7"/>
       <c r="B86" s="54">
         <v>48</v>
@@ -5298,7 +5317,7 @@
       <c r="Z86" s="7"/>
       <c r="AA86" s="7"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="87" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="87" customHeight="1" ht="19.5">
       <c r="A87" s="7"/>
       <c r="B87" s="54">
         <v>49</v>
@@ -5339,7 +5358,7 @@
       <c r="Z87" s="7"/>
       <c r="AA87" s="7"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="88" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="88" customHeight="1" ht="19.5">
       <c r="A88" s="7"/>
       <c r="B88" s="54">
         <v>50</v>
@@ -5380,7 +5399,7 @@
       <c r="Z88" s="7"/>
       <c r="AA88" s="7"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="89" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="89" customHeight="1" ht="19.5">
       <c r="A89" s="7"/>
       <c r="B89" s="140"/>
       <c r="C89" s="123"/>
@@ -5409,7 +5428,7 @@
       <c r="Z89" s="7"/>
       <c r="AA89" s="7"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="90" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="90" customHeight="1" ht="19.5">
       <c r="A90" s="7"/>
       <c r="B90" s="140"/>
       <c r="C90" s="123"/>
@@ -5438,7 +5457,7 @@
       <c r="Z90" s="7"/>
       <c r="AA90" s="7"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="91" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="91" customHeight="1" ht="19.5">
       <c r="A91" s="7"/>
       <c r="B91" s="128"/>
       <c r="C91" s="7"/>
@@ -5467,7 +5486,7 @@
       <c r="Z91" s="7"/>
       <c r="AA91" s="7"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="92" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="92" customHeight="1" ht="19.5">
       <c r="A92" s="7"/>
       <c r="B92" s="128"/>
       <c r="C92" s="7"/>
@@ -5496,7 +5515,7 @@
       <c r="Z92" s="7"/>
       <c r="AA92" s="7"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="93" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="93" customHeight="1" ht="19.5">
       <c r="A93" s="7"/>
       <c r="B93" s="128"/>
       <c r="C93" s="7"/>

</xml_diff>